<commit_message>
quest images + fixed bugs in corpus file
</commit_message>
<xml_diff>
--- a/Experiment 3/Corpus/Corpus2.xlsx
+++ b/Experiment 3/Corpus/Corpus2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\preview_costs\Experiment 3\Corpus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E8CDA3-83D4-457E-8289-A2A974F319E7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8426BA-9B6D-4A26-89B8-BDA45C2F1384}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1349" uniqueCount="911">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="918">
   <si>
     <t>Word</t>
   </si>
@@ -5888,6 +5888,27 @@
   </si>
   <si>
     <t>Was it easy to recover from the recession?</t>
+  </si>
+  <si>
+    <t>contact</t>
+  </si>
+  <si>
+    <t>successful</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>recession</t>
+  </si>
+  <si>
+    <t>forced</t>
+  </si>
+  <si>
+    <t>from</t>
   </si>
 </sst>
 </file>
@@ -6401,9 +6422,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T148"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R143" sqref="R143"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A145" sqref="A145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11914,11 +11935,11 @@
         <v>Yes</v>
       </c>
       <c r="M78" s="14" t="s">
-        <v>158</v>
+        <v>911</v>
       </c>
       <c r="N78" s="14">
         <f t="shared" si="25"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="O78" s="1">
         <f t="shared" si="26"/>
@@ -11931,11 +11952,11 @@
       </c>
       <c r="S78" s="3">
         <f t="shared" si="27"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="T78" s="1">
         <f t="shared" si="28"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:20" x14ac:dyDescent="0.3">
@@ -15453,11 +15474,11 @@
         <v>669</v>
       </c>
       <c r="N130" s="11">
-        <f t="shared" ref="N130:N139" si="44">LEN(M130)</f>
+        <f t="shared" ref="N130:N145" si="44">LEN(M130)</f>
         <v>5</v>
       </c>
       <c r="O130" s="14">
-        <f t="shared" ref="O130:O139" si="45">LEN(C130)</f>
+        <f t="shared" ref="O130:O145" si="45">LEN(C130)</f>
         <v>5</v>
       </c>
       <c r="P130" s="13"/>
@@ -15466,11 +15487,11 @@
         <v>0</v>
       </c>
       <c r="S130" s="3">
-        <f t="shared" ref="S130:S139" si="46">IF(ISBLANK(LEFT(I130,FIND(M130,I130)-1)),0,LEN(TRIM(LEFT(I130,FIND(M130,I130)-1)))-LEN(SUBSTITUTE(LEFT(I130,FIND(M130,I130)-1)," ",""))+1)+1</f>
+        <f t="shared" ref="S130:S145" si="46">IF(ISBLANK(LEFT(I130,FIND(M130,I130)-1)),0,LEN(TRIM(LEFT(I130,FIND(M130,I130)-1)))-LEN(SUBSTITUTE(LEFT(I130,FIND(M130,I130)-1)," ",""))+1)+1</f>
         <v>4</v>
       </c>
       <c r="T130" s="1">
-        <f t="shared" ref="T130:T139" si="47">S130+1</f>
+        <f t="shared" ref="T130:T146" si="47">S130+1</f>
         <v>5</v>
       </c>
     </row>
@@ -16105,9 +16126,17 @@
       <c r="J140" s="12"/>
       <c r="K140" s="12"/>
       <c r="L140" s="5"/>
-      <c r="M140" s="11"/>
-      <c r="N140" s="11"/>
-      <c r="O140" s="1"/>
+      <c r="M140" s="11" t="s">
+        <v>912</v>
+      </c>
+      <c r="N140" s="11">
+        <f t="shared" si="44"/>
+        <v>10</v>
+      </c>
+      <c r="O140" s="1">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
       <c r="P140" s="13" t="s">
         <v>908</v>
       </c>
@@ -16117,8 +16146,14 @@
       <c r="R140" s="12">
         <v>1</v>
       </c>
-      <c r="S140" s="3"/>
-      <c r="T140" s="1"/>
+      <c r="S140" s="3">
+        <f t="shared" si="46"/>
+        <v>9</v>
+      </c>
+      <c r="T140" s="1">
+        <f t="shared" si="47"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="141" spans="1:20" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A141">
@@ -16139,9 +16174,17 @@
       <c r="J141" s="12"/>
       <c r="K141" s="12"/>
       <c r="L141" s="5"/>
-      <c r="M141" s="11"/>
-      <c r="N141" s="11"/>
-      <c r="O141" s="1"/>
+      <c r="M141" s="11" t="s">
+        <v>913</v>
+      </c>
+      <c r="N141" s="11">
+        <f t="shared" si="44"/>
+        <v>2</v>
+      </c>
+      <c r="O141" s="1">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
       <c r="P141" s="13" t="s">
         <v>909</v>
       </c>
@@ -16151,8 +16194,14 @@
       <c r="R141" s="12">
         <v>1</v>
       </c>
-      <c r="S141" s="3"/>
-      <c r="T141" s="1"/>
+      <c r="S141" s="3">
+        <f t="shared" si="46"/>
+        <v>8</v>
+      </c>
+      <c r="T141" s="1">
+        <f t="shared" si="47"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="142" spans="1:20" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A142">
@@ -16173,14 +16222,30 @@
       <c r="J142" s="12"/>
       <c r="K142" s="12"/>
       <c r="L142" s="5"/>
-      <c r="M142" s="11"/>
-      <c r="N142" s="11"/>
-      <c r="O142" s="1"/>
+      <c r="M142" s="11" t="s">
+        <v>914</v>
+      </c>
+      <c r="N142" s="11">
+        <f t="shared" si="44"/>
+        <v>3</v>
+      </c>
+      <c r="O142" s="1">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
       <c r="P142" s="13"/>
       <c r="Q142" s="12"/>
-      <c r="R142" s="12"/>
-      <c r="S142" s="3"/>
-      <c r="T142" s="1"/>
+      <c r="R142" s="12">
+        <v>0</v>
+      </c>
+      <c r="S142" s="3">
+        <f t="shared" si="46"/>
+        <v>7</v>
+      </c>
+      <c r="T142" s="1">
+        <f t="shared" si="47"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="143" spans="1:20" s="17" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A143">
@@ -16201,9 +16266,17 @@
       <c r="J143" s="12"/>
       <c r="K143" s="12"/>
       <c r="L143" s="5"/>
-      <c r="M143" s="11"/>
-      <c r="N143" s="11"/>
-      <c r="O143" s="1"/>
+      <c r="M143" s="11" t="s">
+        <v>915</v>
+      </c>
+      <c r="N143" s="11">
+        <f t="shared" si="44"/>
+        <v>9</v>
+      </c>
+      <c r="O143" s="1">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
       <c r="P143" s="13" t="s">
         <v>910</v>
       </c>
@@ -16213,8 +16286,14 @@
       <c r="R143" s="12">
         <v>1</v>
       </c>
-      <c r="S143" s="3"/>
-      <c r="T143" s="1"/>
+      <c r="S143" s="3">
+        <f t="shared" si="46"/>
+        <v>4</v>
+      </c>
+      <c r="T143" s="1">
+        <f t="shared" si="47"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="144" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A144">
@@ -16226,8 +16305,30 @@
       <c r="I144" s="20" t="s">
         <v>906</v>
       </c>
-    </row>
-    <row r="145" spans="1:15" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="M144" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="N144" s="11">
+        <f t="shared" si="44"/>
+        <v>6</v>
+      </c>
+      <c r="O144" s="1">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="R144" s="3">
+        <v>0</v>
+      </c>
+      <c r="S144" s="3">
+        <f t="shared" si="46"/>
+        <v>5</v>
+      </c>
+      <c r="T144" s="1">
+        <f t="shared" si="47"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="145" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>144</v>
       </c>
@@ -16237,8 +16338,33 @@
       <c r="I145" s="20" t="s">
         <v>907</v>
       </c>
-    </row>
-    <row r="147" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="M145" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="N145" s="11">
+        <f t="shared" si="44"/>
+        <v>4</v>
+      </c>
+      <c r="O145" s="1">
+        <f t="shared" si="45"/>
+        <v>0</v>
+      </c>
+      <c r="R145" s="3">
+        <v>0</v>
+      </c>
+      <c r="S145" s="3">
+        <f t="shared" si="46"/>
+        <v>6</v>
+      </c>
+      <c r="T145" s="1">
+        <f t="shared" si="47"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="146" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="T146" s="1"/>
+    </row>
+    <row r="147" spans="1:20" x14ac:dyDescent="0.3">
       <c r="F147" s="1">
         <f>AVERAGE(F2:F139)</f>
         <v>4.77536231884058</v>
@@ -16260,10 +16386,10 @@
         <v>6</v>
       </c>
     </row>
-    <row r="148" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.3">
       <c r="N148" s="1">
         <f>STDEV(N2:N139)</f>
-        <v>1.2734004533899557</v>
+        <v>1.2709682148307737</v>
       </c>
       <c r="O148" s="1">
         <f>STDEV(O2:O139)</f>
@@ -16280,7 +16406,7 @@
       <formula>4</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N28:N143">
+  <conditionalFormatting sqref="N28:N145">
     <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
       <formula>8</formula>
     </cfRule>

</xml_diff>